<commit_message>
Uncommented code Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ExecutionTestData\Batch1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -478,30 +478,12 @@
   <si>
     <t>121212</t>
   </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_11.0.0_765c8</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyFold_Android_9.0.0_d69de</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyJ8_Android_10.0.0_882d2</t>
-  </si>
-  <si>
-    <t>10.0.0</t>
-  </si>
-  <si>
-    <t>12.0.0</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,16 +528,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -631,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -681,56 +653,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC4125"/>
-          <bgColor rgb="FFCC4125"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC4125"/>
-          <bgColor rgb="FFCC4125"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1232,152 +1169,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:U2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="8" max="21" width="17.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="T1" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q2" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="S2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1387,192 +1213,30 @@
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="U5" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1582,62 +1246,8 @@
       <c r="C6" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="T6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1647,62 +1257,8 @@
       <c r="C7" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1712,62 +1268,8 @@
       <c r="C8" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
@@ -1777,62 +1279,8 @@
       <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
-        <v>3</v>
-      </c>
-      <c r="E9" s="18">
-        <v>4</v>
-      </c>
-      <c r="F9" s="18">
-        <v>5</v>
-      </c>
-      <c r="G9" s="18">
-        <v>6</v>
-      </c>
-      <c r="H9" s="18">
-        <v>7</v>
-      </c>
-      <c r="I9" s="18">
-        <v>8</v>
-      </c>
-      <c r="J9" s="18">
-        <v>9</v>
-      </c>
-      <c r="K9" s="18">
-        <v>10</v>
-      </c>
-      <c r="L9" s="18">
-        <v>11</v>
-      </c>
-      <c r="M9" s="18">
-        <v>12</v>
-      </c>
-      <c r="N9" s="18">
-        <v>13</v>
-      </c>
-      <c r="O9" s="18">
-        <v>14</v>
-      </c>
-      <c r="P9" s="18">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>16</v>
-      </c>
-      <c r="R9" s="18">
-        <v>17</v>
-      </c>
-      <c r="S9" s="18">
-        <v>18</v>
-      </c>
-      <c r="T9" s="18">
-        <v>19</v>
-      </c>
-      <c r="U9" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
@@ -1842,69 +1290,15 @@
       <c r="C10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U2">
-    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="Working">
+  <conditionalFormatting sqref="B2:C2">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Working">
       <formula>LEFT((B2),LEN("Working"))=("Working")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U2">
-    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="Not Working">
+  <conditionalFormatting sqref="B2:C2">
+    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Not Working">
       <formula>LEFT((B2),LEN("Not Working"))=("Not Working")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2008,7 +1402,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -2073,7 +1467,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -2189,7 +1583,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
@@ -2215,7 +1609,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="23"/>
       <c r="B13">
         <v>121212</v>
       </c>

</xml_diff>

<commit_message>
CronJob Shell Script Testing. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\finalList9Feb\batches\Batch1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -478,27 +478,12 @@
   <si>
     <t>121212</t>
   </si>
-  <si>
-    <t>SAMSUNG_GalaxyFold_Android_9.0.0_d69de</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyJ8_Android_10.0.0_882d2</t>
-  </si>
-  <si>
-    <t>10.0.0</t>
-  </si>
-  <si>
-    <t>12.0.0</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,16 +528,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -628,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,8 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1195,22 +1168,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="8" max="21" width="17.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
@@ -1220,62 +1190,8 @@
       <c r="C1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="S1" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="T1" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -1285,62 +1201,8 @@
       <c r="C2" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="U2" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1350,62 +1212,8 @@
       <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -1415,62 +1223,8 @@
       <c r="C4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
@@ -1480,62 +1234,8 @@
       <c r="C5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="R5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1545,62 +1245,8 @@
       <c r="C6" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="T6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1610,62 +1256,8 @@
       <c r="C7" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1675,62 +1267,8 @@
       <c r="C8" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
@@ -1740,62 +1278,8 @@
       <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
-        <v>3</v>
-      </c>
-      <c r="E9" s="18">
-        <v>4</v>
-      </c>
-      <c r="F9" s="18">
-        <v>5</v>
-      </c>
-      <c r="G9" s="18">
-        <v>6</v>
-      </c>
-      <c r="H9" s="18">
-        <v>7</v>
-      </c>
-      <c r="I9" s="18">
-        <v>8</v>
-      </c>
-      <c r="J9" s="18">
-        <v>9</v>
-      </c>
-      <c r="K9" s="18">
-        <v>10</v>
-      </c>
-      <c r="L9" s="18">
-        <v>11</v>
-      </c>
-      <c r="M9" s="18">
-        <v>12</v>
-      </c>
-      <c r="N9" s="18">
-        <v>13</v>
-      </c>
-      <c r="O9" s="18">
-        <v>14</v>
-      </c>
-      <c r="P9" s="18">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>16</v>
-      </c>
-      <c r="R9" s="18">
-        <v>17</v>
-      </c>
-      <c r="S9" s="18">
-        <v>18</v>
-      </c>
-      <c r="T9" s="18">
-        <v>19</v>
-      </c>
-      <c r="U9" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
@@ -1805,68 +1289,14 @@
       <c r="C10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U2">
+  <conditionalFormatting sqref="B2:C2">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Working">
       <formula>LEFT((B2),LEN("Working"))=("Working")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U2">
+  <conditionalFormatting sqref="B2:C2">
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Not Working">
       <formula>LEFT((B2),LEN("Not Working"))=("Not Working")</formula>
     </cfRule>
@@ -1971,7 +1401,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -2036,7 +1466,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -2152,7 +1582,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="22" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
@@ -2178,7 +1608,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13">
         <v>121212</v>
       </c>

</xml_diff>

<commit_message>
Test Data Modification. Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\skippedBatch1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="155">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -478,12 +478,39 @@
   <si>
     <t>121212</t>
   </si>
+  <si>
+    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ8_Android_10.0.0_882d2</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>12.0.0</t>
+  </si>
+  <si>
+    <t>ONEPLUS_5_Android_9.0.0_d9e3e</t>
+  </si>
+  <si>
+    <t>ONEPLUS_8T_Android_11.0.0_f37ff</t>
+  </si>
+  <si>
+    <t>ONEPLUS_9_Android_12.0.0_a5ac6</t>
+  </si>
+  <si>
+    <t>REALME_9i_Android_11.0.0_2410</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA72018_Android_10.0.0_ef0ba</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,11 +552,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -545,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -580,21 +602,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,29 +645,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1168,135 +1177,619 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="20"/>
+    <col min="2" max="2" width="37.85546875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="42" style="20" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="17.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="K1" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="E2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="G2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="D3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="D4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="D5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="R5" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="D6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="22" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="D7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="S7" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="D8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="R8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="S8" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="D9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14">
+        <v>4</v>
+      </c>
+      <c r="F9" s="14">
+        <v>5</v>
+      </c>
+      <c r="G9" s="14">
+        <v>6</v>
+      </c>
+      <c r="H9" s="14">
+        <v>7</v>
+      </c>
+      <c r="I9" s="14">
+        <v>8</v>
+      </c>
+      <c r="J9" s="14">
+        <v>9</v>
+      </c>
+      <c r="K9" s="14">
+        <v>10</v>
+      </c>
+      <c r="L9" s="14">
+        <v>11</v>
+      </c>
+      <c r="M9" s="14">
+        <v>12</v>
+      </c>
+      <c r="N9" s="14">
+        <v>13</v>
+      </c>
+      <c r="O9" s="14">
+        <v>14</v>
+      </c>
+      <c r="P9" s="14">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>16</v>
+      </c>
+      <c r="R9" s="14">
+        <v>17</v>
+      </c>
+      <c r="S9" s="14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="22" t="s">
         <v>32</v>
       </c>
+      <c r="D10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="22" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C2">
+  <conditionalFormatting sqref="B2:S2">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Working">
       <formula>LEFT((B2),LEN("Working"))=("Working")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C2">
+  <conditionalFormatting sqref="B2:S2">
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Not Working">
       <formula>LEFT((B2),LEN("Not Working"))=("Not Working")</formula>
     </cfRule>
@@ -1401,7 +1894,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -1466,7 +1959,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="15"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1582,7 +2075,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
@@ -1608,7 +2101,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="16"/>
       <c r="B13">
         <v>121212</v>
       </c>
@@ -1685,327 +2178,327 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="12" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="12" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="12" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="12" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="12" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="12" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
code modification for rerun batch Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\skippedBatch1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="153">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -477,12 +477,6 @@
   </si>
   <si>
     <t>121212</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyJ8_Android_10.0.0_882d2</t>
   </si>
   <si>
     <t>10.0.0</t>
@@ -655,12 +649,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -670,6 +658,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1177,142 +1171,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="20"/>
-    <col min="2" max="2" width="37.85546875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="42" style="20" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="17.140625" style="20"/>
+    <col min="1" max="1" width="17.140625" style="18"/>
+    <col min="2" max="2" width="37.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="18" customWidth="1"/>
+    <col min="5" max="7" width="17.140625" style="18"/>
+    <col min="8" max="8" width="42.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="18"/>
+    <col min="12" max="12" width="43" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="17.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="H1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="19" t="s">
+      <c r="K1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="E2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="P1" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="17" t="s">
+      <c r="J2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="M2" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1351,322 +1315,214 @@
       <c r="M3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="H4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="J4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="20" t="s">
+      <c r="K4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="M4" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="N5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="P6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="R6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="S6" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q7" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="S7" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="N8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="O8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="S8" s="22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="14">
@@ -1705,91 +1561,55 @@
       <c r="M9" s="14">
         <v>12</v>
       </c>
-      <c r="N9" s="14">
-        <v>13</v>
-      </c>
-      <c r="O9" s="14">
-        <v>14</v>
-      </c>
-      <c r="P9" s="14">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="14">
-        <v>16</v>
-      </c>
-      <c r="R9" s="14">
-        <v>17</v>
-      </c>
-      <c r="S9" s="14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="L10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="S10" s="22" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:S2">
+  <conditionalFormatting sqref="B2:M2">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Working">
       <formula>LEFT((B2),LEN("Working"))=("Working")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:S2">
+  <conditionalFormatting sqref="B2:M2">
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Not Working">
       <formula>LEFT((B2),LEN("Not Working"))=("Not Working")</formula>
     </cfRule>
@@ -1894,7 +1714,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
@@ -1959,7 +1779,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -2075,7 +1895,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="22" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
@@ -2101,7 +1921,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="22"/>
       <c r="B13">
         <v>121212</v>
       </c>

</xml_diff>

<commit_message>
Test data Updation Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shafqat.ali\Desktop\jaya credential batches\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shafqat.ali\Desktop\jaya credential batches\rerun batches\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>OPPO_A53_Android_10.0.0_bd07c</t>
   </si>
   <si>
-    <t>11.0.0</t>
-  </si>
-  <si>
     <t>EndPoint</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   </si>
   <si>
     <t>9.0.0</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ4Plus_Android_9.0.0_94cc6</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1073,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -1123,7 +1123,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,10 +1186,10 @@
         <v>19</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1219,10 +1219,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -1233,10 +1233,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -1247,10 +1247,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,10 +1258,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>